<commit_message>
subiendo lista de archivos objetados
</commit_message>
<xml_diff>
--- a/archivos_para_importacion/objetados.xlsx
+++ b/archivos_para_importacion/objetados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="270">
   <si>
     <t xml:space="preserve">CUE</t>
   </si>
@@ -803,6 +803,33 @@
   </si>
   <si>
     <t xml:space="preserve">ECA86B1E3755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000670438a263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6650A9C5AD9F19627421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7427EA97CE37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C03FD5287B07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61E48A760302DF984B08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C03FD5177126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7427EA9082A8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C03FD52891A8</t>
   </si>
 </sst>
 </file>
@@ -813,7 +840,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -839,6 +866,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -885,7 +920,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -918,6 +953,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -935,13 +982,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A153" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71:F173"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A162" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B178" activeCellId="0" sqref="B178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.3"/>
@@ -4812,6 +4859,122 @@
       </c>
       <c r="H173" s="0"/>
     </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="8" t="n">
+        <v>60793500</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E174" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G174" s="3"/>
+      <c r="H174" s="0"/>
+      <c r="I174" s="9"/>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="8" t="n">
+        <v>60793500</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C175" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E175" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F175" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G175" s="3"/>
+      <c r="H175" s="0"/>
+      <c r="I175" s="9"/>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="8" t="n">
+        <v>60793500</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D176" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E176" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F176" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G176" s="3"/>
+      <c r="H176" s="0"/>
+      <c r="I176" s="9"/>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="n">
+        <v>60793500</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C177" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E177" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F177" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G177" s="3"/>
+      <c r="H177" s="0"/>
+      <c r="I177" s="9"/>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="8" t="n">
+        <v>60793500</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C178" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E178" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F178" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G178" s="3"/>
+      <c r="H178" s="0"/>
+      <c r="I178" s="9"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>